<commit_message>
Tratamento de materiais parte 1
</commit_message>
<xml_diff>
--- a/estoque.XLSX
+++ b/estoque.XLSX
@@ -1753,10 +1753,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="2">
-        <v>340.000</v>
+        <v>417.000</v>
       </c>
       <c r="H2" s="3">
-        <v>1230.14</v>
+        <v>1508.71</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1779,10 +1779,10 @@
         <v>5</v>
       </c>
       <c r="G3" s="2">
-        <v>1951.000</v>
+        <v>1866.000</v>
       </c>
       <c r="H3" s="3">
-        <v>255703.67</v>
+        <v>244563.86</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1987,10 +1987,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="2">
-        <v>3998.000</v>
+        <v>3984.000</v>
       </c>
       <c r="H11" s="3">
-        <v>122657.28</v>
+        <v>122227.77</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2013,10 +2013,10 @@
         <v>5</v>
       </c>
       <c r="G12" s="2">
-        <v>58.000</v>
+        <v>78.000</v>
       </c>
       <c r="H12" s="3">
-        <v>4952.64</v>
+        <v>6660.45</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2117,10 +2117,10 @@
         <v>5</v>
       </c>
       <c r="G16" s="2">
-        <v>1671.000</v>
+        <v>1639.000</v>
       </c>
       <c r="H16" s="3">
-        <v>142816.28</v>
+        <v>140081.29</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2221,10 +2221,10 @@
         <v>5</v>
       </c>
       <c r="G20" s="2">
-        <v>2395.000</v>
+        <v>2663.000</v>
       </c>
       <c r="H20" s="3">
-        <v>202717.53</v>
+        <v>225401.66</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2299,10 +2299,10 @@
         <v>5</v>
       </c>
       <c r="G23" s="2">
-        <v>66.000</v>
+        <v>67.000</v>
       </c>
       <c r="H23" s="3">
-        <v>9633.90</v>
+        <v>9779.87</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2325,10 +2325,10 @@
         <v>5</v>
       </c>
       <c r="G24" s="2">
-        <v>133.000</v>
+        <v>149.000</v>
       </c>
       <c r="H24" s="3">
-        <v>60119.05</v>
+        <v>67351.70</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2429,10 +2429,10 @@
         <v>52</v>
       </c>
       <c r="G28" s="2">
-        <v>294.480</v>
+        <v>469.480</v>
       </c>
       <c r="H28" s="3">
-        <v>11144.53</v>
+        <v>17748.73</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2455,10 +2455,10 @@
         <v>52</v>
       </c>
       <c r="G29" s="2">
-        <v>193.890</v>
+        <v>192.890</v>
       </c>
       <c r="H29" s="3">
-        <v>4970.02</v>
+        <v>4944.38</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2481,10 +2481,10 @@
         <v>52</v>
       </c>
       <c r="G30" s="2">
-        <v>754.600</v>
+        <v>620.600</v>
       </c>
       <c r="H30" s="3">
-        <v>8837.42</v>
+        <v>7268.09</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2585,10 +2585,10 @@
         <v>5</v>
       </c>
       <c r="G34" s="2">
-        <v>289.000</v>
+        <v>286.000</v>
       </c>
       <c r="H34" s="3">
-        <v>5362.39</v>
+        <v>5306.73</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2871,10 +2871,10 @@
         <v>5</v>
       </c>
       <c r="G45" s="2">
-        <v>9.000</v>
+        <v>10.000</v>
       </c>
       <c r="H45" s="3">
-        <v>878.23</v>
+        <v>975.81</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2975,10 +2975,10 @@
         <v>5</v>
       </c>
       <c r="G49" s="2">
-        <v>16.000</v>
+        <v>22.000</v>
       </c>
       <c r="H49" s="3">
-        <v>1767.79</v>
+        <v>2430.71</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3027,10 +3027,10 @@
         <v>5</v>
       </c>
       <c r="G51" s="2">
-        <v>1.000</v>
+        <v>4.000</v>
       </c>
       <c r="H51" s="3">
-        <v>57.33</v>
+        <v>229.34</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3131,10 +3131,10 @@
         <v>52</v>
       </c>
       <c r="G55" s="2">
-        <v>199.900</v>
+        <v>195.900</v>
       </c>
       <c r="H55" s="3">
-        <v>4118.18</v>
+        <v>4208.31</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3264,7 +3264,7 @@
         <v>1.000</v>
       </c>
       <c r="H60" s="3">
-        <v>3608.81</v>
+        <v>3716.19</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -3290,7 +3290,7 @@
         <v>1.000</v>
       </c>
       <c r="H61" s="3">
-        <v>1676.79</v>
+        <v>1707.25</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -3313,10 +3313,10 @@
         <v>5</v>
       </c>
       <c r="G62" s="2">
-        <v>10.000</v>
+        <v>14.000</v>
       </c>
       <c r="H62" s="3">
-        <v>5661.51</v>
+        <v>7926.11</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -3573,10 +3573,10 @@
         <v>5</v>
       </c>
       <c r="G72" s="2">
-        <v>382.000</v>
+        <v>441.000</v>
       </c>
       <c r="H72" s="3">
-        <v>8605.07</v>
+        <v>9934.13</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3677,10 +3677,10 @@
         <v>5</v>
       </c>
       <c r="G76" s="2">
-        <v>17.000</v>
+        <v>16.000</v>
       </c>
       <c r="H76" s="3">
-        <v>1025.55</v>
+        <v>965.23</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3703,10 +3703,10 @@
         <v>5</v>
       </c>
       <c r="G77" s="2">
-        <v>1.000</v>
+        <v>2.000</v>
       </c>
       <c r="H77" s="3">
-        <v>23.34</v>
+        <v>46.69</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3758,7 +3758,7 @@
         <v>62.000</v>
       </c>
       <c r="H79" s="3">
-        <v>11239.67</v>
+        <v>11556.75</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3784,7 +3784,7 @@
         <v>317.000</v>
       </c>
       <c r="H80" s="3">
-        <v>5495.56</v>
+        <v>5495.51</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3963,10 +3963,10 @@
         <v>5</v>
       </c>
       <c r="G87" s="2">
-        <v>3996.000</v>
+        <v>4024.000</v>
       </c>
       <c r="H87" s="3">
-        <v>72888.35</v>
+        <v>73399.08</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4171,10 +4171,10 @@
         <v>5</v>
       </c>
       <c r="G95" s="2">
-        <v>24.000</v>
+        <v>27.000</v>
       </c>
       <c r="H95" s="3">
-        <v>365.03</v>
+        <v>410.66</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -4197,10 +4197,10 @@
         <v>5</v>
       </c>
       <c r="G96" s="2">
-        <v>134.000</v>
+        <v>116.000</v>
       </c>
       <c r="H96" s="3">
-        <v>765.43</v>
+        <v>662.62</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -4353,10 +4353,10 @@
         <v>5</v>
       </c>
       <c r="G102" s="2">
-        <v>42.000</v>
+        <v>46.000</v>
       </c>
       <c r="H102" s="3">
-        <v>5520.65</v>
+        <v>6046.42</v>
       </c>
     </row>
     <row r="103" spans="1:8">
@@ -4382,7 +4382,7 @@
         <v>44.000</v>
       </c>
       <c r="H103" s="3">
-        <v>3803.62</v>
+        <v>3803.61</v>
       </c>
     </row>
     <row r="104" spans="1:8">
@@ -4483,10 +4483,10 @@
         <v>5</v>
       </c>
       <c r="G107" s="2">
-        <v>329.000</v>
+        <v>429.000</v>
       </c>
       <c r="H107" s="3">
-        <v>1388.75</v>
+        <v>1810.86</v>
       </c>
     </row>
     <row r="108" spans="1:8">
@@ -4509,10 +4509,10 @@
         <v>5</v>
       </c>
       <c r="G108" s="2">
-        <v>35.000</v>
+        <v>40.000</v>
       </c>
       <c r="H108" s="3">
-        <v>981.38</v>
+        <v>1106.48</v>
       </c>
     </row>
     <row r="109" spans="1:8">
@@ -4535,10 +4535,10 @@
         <v>5</v>
       </c>
       <c r="G109" s="2">
-        <v>46.000</v>
+        <v>44.000</v>
       </c>
       <c r="H109" s="3">
-        <v>1553.15</v>
+        <v>1485.62</v>
       </c>
     </row>
     <row r="110" spans="1:8">
@@ -4564,7 +4564,7 @@
         <v>112.000</v>
       </c>
       <c r="H110" s="3">
-        <v>5565.90</v>
+        <v>5565.89</v>
       </c>
     </row>
     <row r="111" spans="1:8">
@@ -4587,10 +4587,10 @@
         <v>5</v>
       </c>
       <c r="G111" s="2">
-        <v>162.000</v>
+        <v>177.000</v>
       </c>
       <c r="H111" s="3">
-        <v>5793.96</v>
+        <v>6562.07</v>
       </c>
     </row>
     <row r="112" spans="1:8">
@@ -4873,10 +4873,10 @@
         <v>5</v>
       </c>
       <c r="G122" s="2">
-        <v>1.000</v>
+        <v>3.000</v>
       </c>
       <c r="H122" s="3">
-        <v>151.60</v>
+        <v>454.82</v>
       </c>
     </row>
     <row r="123" spans="1:8">
@@ -4925,10 +4925,10 @@
         <v>5</v>
       </c>
       <c r="G124" s="2">
-        <v>4.000</v>
+        <v>5.000</v>
       </c>
       <c r="H124" s="3">
-        <v>114.45</v>
+        <v>143.07</v>
       </c>
     </row>
     <row r="125" spans="1:8">
@@ -4951,10 +4951,10 @@
         <v>5</v>
       </c>
       <c r="G125" s="2">
-        <v>617.000</v>
+        <v>602.000</v>
       </c>
       <c r="H125" s="3">
-        <v>3471.97</v>
+        <v>3387.57</v>
       </c>
     </row>
     <row r="126" spans="1:8">
@@ -5029,10 +5029,10 @@
         <v>5</v>
       </c>
       <c r="G128" s="2">
-        <v>4.000</v>
+        <v>7.000</v>
       </c>
       <c r="H128" s="3">
-        <v>991.91</v>
+        <v>1735.84</v>
       </c>
     </row>
     <row r="129" spans="1:8">
@@ -5055,10 +5055,10 @@
         <v>5</v>
       </c>
       <c r="G129" s="2">
-        <v>22.000</v>
+        <v>24.000</v>
       </c>
       <c r="H129" s="3">
-        <v>2281.65</v>
+        <v>2489.07</v>
       </c>
     </row>
     <row r="130" spans="1:8">
@@ -5159,10 +5159,10 @@
         <v>5</v>
       </c>
       <c r="G133" s="2">
-        <v>17.000</v>
+        <v>27.000</v>
       </c>
       <c r="H133" s="3">
-        <v>3293.85</v>
+        <v>5231.40</v>
       </c>
     </row>
     <row r="134" spans="1:8">
@@ -5240,7 +5240,7 @@
         <v>251.000</v>
       </c>
       <c r="H136" s="3">
-        <v>84289.12</v>
+        <v>84289.17</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5263,10 +5263,10 @@
         <v>5</v>
       </c>
       <c r="G137" s="2">
-        <v>175.000</v>
+        <v>174.000</v>
       </c>
       <c r="H137" s="3">
-        <v>27744.96</v>
+        <v>27586.42</v>
       </c>
     </row>
     <row r="138" spans="1:8">
@@ -5341,10 +5341,10 @@
         <v>5</v>
       </c>
       <c r="G140" s="2">
-        <v>195.000</v>
+        <v>194.000</v>
       </c>
       <c r="H140" s="3">
-        <v>9160.07</v>
+        <v>9113.09</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -6202,7 +6202,7 @@
         <v>185.000</v>
       </c>
       <c r="H173" s="3">
-        <v>6973.57</v>
+        <v>6973.58</v>
       </c>
     </row>
     <row r="174" spans="1:8">
@@ -6251,10 +6251,10 @@
         <v>5</v>
       </c>
       <c r="G175" s="2">
-        <v>188.000</v>
+        <v>230.000</v>
       </c>
       <c r="H175" s="3">
-        <v>32444.93</v>
+        <v>39693.26</v>
       </c>
     </row>
     <row r="176" spans="1:8">
@@ -6277,10 +6277,10 @@
         <v>5</v>
       </c>
       <c r="G176" s="2">
-        <v>219.000</v>
+        <v>262.000</v>
       </c>
       <c r="H176" s="3">
-        <v>7150.19</v>
+        <v>8755.57</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6407,10 +6407,10 @@
         <v>5</v>
       </c>
       <c r="G181" s="2">
-        <v>5.000</v>
+        <v>10.000</v>
       </c>
       <c r="H181" s="3">
-        <v>187.08</v>
+        <v>374.15</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6540,7 +6540,7 @@
         <v>53.000</v>
       </c>
       <c r="H186" s="3">
-        <v>2078.03</v>
+        <v>2079.32</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6563,10 +6563,10 @@
         <v>5</v>
       </c>
       <c r="G187" s="2">
-        <v>338.000</v>
+        <v>455.000</v>
       </c>
       <c r="H187" s="3">
-        <v>2435.13</v>
+        <v>3278.07</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6615,10 +6615,10 @@
         <v>5</v>
       </c>
       <c r="G189" s="2">
-        <v>800.000</v>
+        <v>781.000</v>
       </c>
       <c r="H189" s="3">
-        <v>5390.45</v>
+        <v>5262.42</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6693,10 +6693,10 @@
         <v>5</v>
       </c>
       <c r="G192" s="2">
-        <v>3267.000</v>
+        <v>3461.000</v>
       </c>
       <c r="H192" s="3">
-        <v>32843.80</v>
+        <v>34794.15</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6901,10 +6901,10 @@
         <v>5</v>
       </c>
       <c r="G200" s="2">
-        <v>22.000</v>
+        <v>23.000</v>
       </c>
       <c r="H200" s="3">
-        <v>11011.15</v>
+        <v>11511.66</v>
       </c>
     </row>
     <row r="201" spans="1:8">
@@ -7161,10 +7161,10 @@
         <v>5</v>
       </c>
       <c r="G210" s="2">
-        <v>146.000</v>
+        <v>141.000</v>
       </c>
       <c r="H210" s="3">
-        <v>197.27</v>
+        <v>190.52</v>
       </c>
     </row>
     <row r="211" spans="1:8">
@@ -7187,10 +7187,10 @@
         <v>52</v>
       </c>
       <c r="G211" s="2">
-        <v>68565.000</v>
+        <v>69575.000</v>
       </c>
       <c r="H211" s="3">
-        <v>160735.93</v>
+        <v>163103.72</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7239,10 +7239,10 @@
         <v>5</v>
       </c>
       <c r="G213" s="2">
-        <v>72.000</v>
+        <v>80.000</v>
       </c>
       <c r="H213" s="3">
-        <v>2566.36</v>
+        <v>2851.51</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7372,7 +7372,7 @@
         <v>74.000</v>
       </c>
       <c r="H218" s="3">
-        <v>1180.84</v>
+        <v>1181.25</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7424,7 +7424,7 @@
         <v>16.000</v>
       </c>
       <c r="H220" s="3">
-        <v>1909.36</v>
+        <v>2387.60</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7447,10 +7447,10 @@
         <v>5</v>
       </c>
       <c r="G221" s="2">
-        <v>284.000</v>
+        <v>288.000</v>
       </c>
       <c r="H221" s="3">
-        <v>14978.21</v>
+        <v>15189.17</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7473,10 +7473,10 @@
         <v>5</v>
       </c>
       <c r="G222" s="2">
-        <v>5973.000</v>
+        <v>6082.000</v>
       </c>
       <c r="H222" s="3">
-        <v>50532.55</v>
+        <v>51454.54</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7551,10 +7551,10 @@
         <v>5</v>
       </c>
       <c r="G225" s="2">
-        <v>89.000</v>
+        <v>101.000</v>
       </c>
       <c r="H225" s="3">
-        <v>24385.55</v>
+        <v>27673.49</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7655,10 +7655,10 @@
         <v>5</v>
       </c>
       <c r="G229" s="2">
-        <v>176.000</v>
+        <v>194.000</v>
       </c>
       <c r="H229" s="3">
-        <v>12540.84</v>
+        <v>13823.42</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -7863,10 +7863,10 @@
         <v>5</v>
       </c>
       <c r="G237" s="2">
-        <v>6.000</v>
+        <v>5.000</v>
       </c>
       <c r="H237" s="3">
-        <v>154.79</v>
+        <v>128.99</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -7915,10 +7915,10 @@
         <v>5</v>
       </c>
       <c r="G239" s="2">
-        <v>83.000</v>
+        <v>85.000</v>
       </c>
       <c r="H239" s="3">
-        <v>7856.29</v>
+        <v>8045.60</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -7944,7 +7944,7 @@
         <v>57.000</v>
       </c>
       <c r="H240" s="3">
-        <v>4990.32</v>
+        <v>5429.83</v>
       </c>
     </row>
     <row r="241" spans="1:8">
@@ -8071,10 +8071,10 @@
         <v>5</v>
       </c>
       <c r="G245" s="2">
-        <v>18.000</v>
+        <v>19.000</v>
       </c>
       <c r="H245" s="3">
-        <v>2360.52</v>
+        <v>2491.66</v>
       </c>
     </row>
     <row r="246" spans="1:8">
@@ -8332,7 +8332,7 @@
       </c>
       <c r="G255" s="5"/>
       <c r="H255" s="6">
-        <v>2273695.07</v>
+        <v>2328355.94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajuste de materiais match pt1
</commit_message>
<xml_diff>
--- a/estoque.XLSX
+++ b/estoque.XLSX
@@ -1753,10 +1753,10 @@
         <v>5</v>
       </c>
       <c r="G2" s="2">
-        <v>417.000</v>
+        <v>264.000</v>
       </c>
       <c r="H2" s="3">
-        <v>1508.71</v>
+        <v>955.15</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1779,10 +1779,10 @@
         <v>5</v>
       </c>
       <c r="G3" s="2">
-        <v>1866.000</v>
+        <v>1725.000</v>
       </c>
       <c r="H3" s="3">
-        <v>244563.86</v>
+        <v>233235.85</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1987,10 +1987,10 @@
         <v>5</v>
       </c>
       <c r="G11" s="2">
-        <v>3984.000</v>
+        <v>3983.000</v>
       </c>
       <c r="H11" s="3">
-        <v>122227.77</v>
+        <v>122197.09</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2117,10 +2117,10 @@
         <v>5</v>
       </c>
       <c r="G16" s="2">
-        <v>1639.000</v>
+        <v>1632.000</v>
       </c>
       <c r="H16" s="3">
-        <v>140081.29</v>
+        <v>139483.01</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2221,10 +2221,10 @@
         <v>5</v>
       </c>
       <c r="G20" s="2">
-        <v>2663.000</v>
+        <v>2652.000</v>
       </c>
       <c r="H20" s="3">
-        <v>225401.66</v>
+        <v>224470.60</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2484,7 +2484,7 @@
         <v>620.600</v>
       </c>
       <c r="H30" s="3">
-        <v>7268.09</v>
+        <v>7194.42</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -3576,7 +3576,7 @@
         <v>441.000</v>
       </c>
       <c r="H72" s="3">
-        <v>9934.13</v>
+        <v>9934.12</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3963,10 +3963,10 @@
         <v>5</v>
       </c>
       <c r="G87" s="2">
-        <v>4024.000</v>
+        <v>4019.000</v>
       </c>
       <c r="H87" s="3">
-        <v>73399.08</v>
+        <v>73307.88</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -5237,10 +5237,10 @@
         <v>5</v>
       </c>
       <c r="G136" s="2">
-        <v>251.000</v>
+        <v>249.000</v>
       </c>
       <c r="H136" s="3">
-        <v>84289.17</v>
+        <v>83617.55</v>
       </c>
     </row>
     <row r="137" spans="1:8">
@@ -5341,10 +5341,10 @@
         <v>5</v>
       </c>
       <c r="G140" s="2">
-        <v>194.000</v>
+        <v>191.000</v>
       </c>
       <c r="H140" s="3">
-        <v>9113.09</v>
+        <v>8972.17</v>
       </c>
     </row>
     <row r="141" spans="1:8">
@@ -6693,10 +6693,10 @@
         <v>5</v>
       </c>
       <c r="G192" s="2">
-        <v>3461.000</v>
+        <v>3455.000</v>
       </c>
       <c r="H192" s="3">
-        <v>34794.15</v>
+        <v>34733.84</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -7187,10 +7187,10 @@
         <v>52</v>
       </c>
       <c r="G211" s="2">
-        <v>69575.000</v>
+        <v>69534.800</v>
       </c>
       <c r="H211" s="3">
-        <v>163103.72</v>
+        <v>163009.49</v>
       </c>
     </row>
     <row r="212" spans="1:8">
@@ -7473,10 +7473,10 @@
         <v>5</v>
       </c>
       <c r="G222" s="2">
-        <v>6082.000</v>
+        <v>6081.000</v>
       </c>
       <c r="H222" s="3">
-        <v>51454.54</v>
+        <v>51446.08</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -8332,7 +8332,7 @@
       </c>
       <c r="G255" s="5"/>
       <c r="H255" s="6">
-        <v>2328355.94</v>
+        <v>2313773.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>